<commit_message>
added more methods, fixed a few glitches (eg. was reporting 310.1 and 310.1000002).
</commit_message>
<xml_diff>
--- a/3_13_2019_CFR_Methods.xlsx
+++ b/3_13_2019_CFR_Methods.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$158</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$159</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="154">
   <si>
     <t>Char_Name</t>
   </si>
@@ -474,6 +474,21 @@
   </si>
   <si>
     <t>4500-NH3 E</t>
+  </si>
+  <si>
+    <t>608.3</t>
+  </si>
+  <si>
+    <t>310.1</t>
+  </si>
+  <si>
+    <t>300.1</t>
+  </si>
+  <si>
+    <t>525.2</t>
+  </si>
+  <si>
+    <t>150.2</t>
   </si>
 </sst>
 </file>
@@ -814,11 +829,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E158"/>
+  <dimension ref="A1:E159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C154" sqref="C154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,8 +903,8 @@
       <c r="B4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="3">
-        <v>310.10000000000002</v>
+      <c r="C4" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>49</v>
@@ -1500,8 +1515,8 @@
       <c r="B40" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C40" s="3">
-        <v>300.10000000000002</v>
+      <c r="C40" s="3" t="s">
+        <v>151</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>49</v>
@@ -1636,8 +1651,8 @@
       <c r="B48" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C48" s="3">
-        <v>300.10000000000002</v>
+      <c r="C48" s="3" t="s">
+        <v>151</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>49</v>
@@ -1976,8 +1991,8 @@
       <c r="B68" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C68" s="3">
-        <v>525.20000000000005</v>
+      <c r="C68" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>49</v>
@@ -2078,8 +2093,8 @@
       <c r="B74" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C74" s="3">
-        <v>525.20000000000005</v>
+      <c r="C74" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>49</v>
@@ -2571,8 +2586,8 @@
       <c r="B103" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C103" s="3">
-        <v>525.20000000000005</v>
+      <c r="C103" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>49</v>
@@ -2843,8 +2858,8 @@
       <c r="B119" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C119" s="3">
-        <v>150.19999999999999</v>
+      <c r="C119" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>49</v>
@@ -3302,8 +3317,8 @@
       <c r="B146" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C146" s="3">
-        <v>300.10000000000002</v>
+      <c r="C146" s="3" t="s">
+        <v>151</v>
       </c>
       <c r="D146" s="1" t="s">
         <v>49</v>
@@ -3438,8 +3453,8 @@
       <c r="B154" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C154" s="3">
-        <v>525.20000000000005</v>
+      <c r="C154" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="D154" s="1" t="s">
         <v>49</v>
@@ -3450,13 +3465,13 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>142</v>
+        <v>37</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C155" s="3">
-        <v>200.7</v>
+        <v>141</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>149</v>
       </c>
       <c r="D155" s="1" t="s">
         <v>49</v>
@@ -3473,7 +3488,7 @@
         <v>143</v>
       </c>
       <c r="C156" s="3">
-        <v>200.8</v>
+        <v>200.7</v>
       </c>
       <c r="D156" s="1" t="s">
         <v>49</v>
@@ -3489,11 +3504,11 @@
       <c r="B157" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C157" s="3" t="s">
-        <v>76</v>
+      <c r="C157" s="3">
+        <v>200.8</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E157" s="1" t="s">
         <v>144</v>
@@ -3507,17 +3522,34 @@
         <v>143</v>
       </c>
       <c r="C158" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C159" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D158" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E158" s="1" t="s">
+      <c r="D159" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E159" s="1" t="s">
         <v>144</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D158">
+  <autoFilter ref="A1:D159">
     <sortState ref="A2:D272">
       <sortCondition ref="A1:A272"/>
     </sortState>

</xml_diff>

<commit_message>
add a few more CFR methods
</commit_message>
<xml_diff>
--- a/3_13_2019_CFR_Methods.xlsx
+++ b/3_13_2019_CFR_Methods.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$159</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$161</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="155">
   <si>
     <t>Char_Name</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Alkalinity, total</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>7429-90-5</t>
   </si>
   <si>
@@ -489,6 +486,12 @@
   </si>
   <si>
     <t>150.2</t>
+  </si>
+  <si>
+    <t>120.1</t>
+  </si>
+  <si>
+    <t>2340B</t>
   </si>
 </sst>
 </file>
@@ -829,11 +832,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E159"/>
+  <dimension ref="A1:E161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C154" sqref="C154"/>
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E155" sqref="E155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,16 +853,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -873,10 +876,10 @@
         <v>615</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -887,13 +890,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -901,16 +904,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -918,2638 +921,2672 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="3">
         <v>200.7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="3">
         <v>200.8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" s="3">
         <v>350.1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="C18" s="3">
         <v>200.7</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="C19" s="3">
         <v>200.8</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="C20" s="3">
         <v>200.9</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="C21" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C22" s="3">
         <v>200.7</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C23" s="3">
         <v>200.8</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C24" s="3">
         <v>200.9</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="D25" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C28" s="3">
         <v>614</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C29" s="3">
         <v>200.7</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C30" s="3">
         <v>200.8</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="C32" s="3">
         <v>200.7</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="C33" s="3">
         <v>200.8</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="C34" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C35" s="3">
         <v>200.7</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C36" s="3">
         <v>200.8</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="D38" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="C39" s="3">
         <v>300</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="C40" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="C41" s="3">
         <v>200.7</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="C42" s="3">
         <v>200.8</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="C43" s="3">
         <v>200.9</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="C44" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="C45" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B46" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B46" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="C46" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C47" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C48" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C49" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C50" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="C51" s="3">
         <v>200.7</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="C52" s="3">
         <v>200.8</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="C53" s="3">
         <v>200.9</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="C54" s="3">
         <v>218.2</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="C55" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C56" s="3">
         <v>200.7</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C57" s="3">
         <v>200.8</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C59" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="D59" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C60" s="3">
-        <v>200.7</v>
+        <v>49</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="C61" s="3">
-        <v>200.8</v>
+        <v>200.7</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="C62" s="3">
-        <v>200.9</v>
+        <v>200.8</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>55</v>
+      <c r="C63" s="3">
+        <v>200.9</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="C64" s="3" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C65" s="3">
-        <v>335.4</v>
+        <v>85</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>90</v>
+      <c r="C66" s="3">
+        <v>335.4</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>152</v>
+        <v>90</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C70" s="3" t="s">
-        <v>93</v>
+        <v>146</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C71" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C72" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C73" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>152</v>
+        <v>95</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>50</v>
+        <v>97</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C76" s="3">
-        <v>353.2</v>
+        <v>49</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>99</v>
+        <v>49</v>
+      </c>
+      <c r="C77" s="3">
+        <v>353.2</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>100</v>
+        <v>18</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C78" s="3">
-        <v>200.7</v>
+        <v>49</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="C79" s="3">
-        <v>200.8</v>
+        <v>200.7</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>76</v>
+      <c r="C80" s="3">
+        <v>200.8</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="C81" s="3" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C82" s="3">
-        <v>200.7</v>
+        <v>100</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="C83" s="3">
-        <v>200.8</v>
+        <v>200.7</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B84" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="C84" s="3">
-        <v>200.9</v>
+        <v>200.8</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B85" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>76</v>
+      <c r="C85" s="3">
+        <v>200.9</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B86" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="C86" s="3" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="C87" s="3" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C88" s="3">
-        <v>200.7</v>
+        <v>102</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C89" s="3">
-        <v>200.8</v>
+        <v>200.7</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>76</v>
+        <v>19</v>
+      </c>
+      <c r="C90" s="3">
+        <v>200.8</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>21</v>
+        <v>103</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C92" s="3">
-        <v>614</v>
+        <v>19</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>106</v>
+        <v>20</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>22</v>
+        <v>104</v>
       </c>
       <c r="C93" s="3">
-        <v>200.7</v>
+        <v>614</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C94" s="3">
-        <v>200.8</v>
+        <v>200.7</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C95" s="3">
-        <v>1638</v>
+        <v>200.8</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>76</v>
+        <v>21</v>
+      </c>
+      <c r="C96" s="3">
+        <v>1638</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C98" s="3">
-        <v>245.1</v>
+        <v>21</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B99" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="C99" s="3">
-        <v>245.2</v>
+        <v>245.1</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="C100" s="3">
-        <v>245.7</v>
+        <v>245.2</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B101" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>109</v>
+      <c r="C101" s="3">
+        <v>245.7</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="C102" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C102" s="3" t="s">
-        <v>110</v>
-      </c>
       <c r="D102" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>23</v>
+        <v>106</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>152</v>
+        <v>109</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>112</v>
+        <v>22</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C104" s="3">
-        <v>200.7</v>
+        <v>110</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>151</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C105" s="3">
-        <v>200.8</v>
+        <v>200.7</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>55</v>
+        <v>23</v>
+      </c>
+      <c r="C106" s="3">
+        <v>200.8</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C107" s="3">
-        <v>200.7</v>
+        <v>23</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B108" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B108" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="C108" s="3">
-        <v>200.8</v>
+        <v>200.7</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B109" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B109" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>55</v>
+      <c r="C109" s="3">
+        <v>200.8</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>25</v>
+        <v>112</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>147</v>
+        <v>54</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C111" s="3">
-        <v>10206</v>
+        <v>114</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C112" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
+      </c>
+      <c r="C112" s="3">
+        <v>10206</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B113" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C113" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C113" s="3" t="s">
-        <v>117</v>
-      </c>
       <c r="D113" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>50</v>
+        <v>114</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C115" s="3">
-        <v>353.2</v>
+        <v>49</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>118</v>
+        <v>49</v>
+      </c>
+      <c r="C116" s="3">
+        <v>353.2</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>119</v>
+        <v>25</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>27</v>
+        <v>118</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C118" s="3">
-        <v>614</v>
+        <v>49</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>153</v>
+        <v>123</v>
+      </c>
+      <c r="C119" s="3">
+        <v>614</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>125</v>
+        <v>152</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C122" s="3">
-        <v>420.1</v>
+        <v>49</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>127</v>
+        <v>27</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C123" s="3">
-        <v>365.3</v>
+        <v>420.1</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C124" s="3" t="s">
-        <v>122</v>
+        <v>49</v>
+      </c>
+      <c r="C124" s="3">
+        <v>365.3</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C126" s="3">
-        <v>200.7</v>
+        <v>126</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B127" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B127" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="C127" s="3">
-        <v>365.3</v>
+        <v>200.7</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B128" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B128" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="C128" s="3">
-        <v>365.4</v>
+        <v>365.3</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B129" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B129" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C129" s="3" t="s">
-        <v>121</v>
+      <c r="C129" s="3">
+        <v>365.4</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B130" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B130" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="C130" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B131" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B131" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="C131" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B132" s="2">
-        <v>2023695</v>
+        <v>28</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C133" s="3">
-        <v>200.7</v>
+        <v>127</v>
+      </c>
+      <c r="B133" s="2">
+        <v>2023695</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B134" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B134" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="C134" s="3">
-        <v>200.8</v>
+        <v>200.7</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B135" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B135" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="C135" s="3">
-        <v>200.9</v>
+        <v>200.8</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B136" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B136" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C136" s="3" t="s">
-        <v>65</v>
+      <c r="C136" s="3">
+        <v>200.9</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B137" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B137" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="C137" s="3" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C138" s="3">
-        <v>200.7</v>
+        <v>129</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B139" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B139" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="C139" s="3">
-        <v>200.8</v>
+        <v>200.7</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B140" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B140" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="C140" s="3">
-        <v>200.9</v>
+        <v>200.8</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B141" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B141" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C141" s="3" t="s">
-        <v>55</v>
+      <c r="C141" s="3">
+        <v>200.9</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>31</v>
+        <v>130</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C142" s="3">
-        <v>615</v>
+        <v>131</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B143" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B143" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C143" s="3" t="s">
-        <v>51</v>
+      <c r="C143" s="3">
+        <v>615</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>133</v>
+        <v>31</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>146</v>
+        <v>50</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>34</v>
+        <v>132</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B146" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B146" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="C146" s="3" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B147" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B147" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="C147" s="3" t="s">
-        <v>78</v>
+        <v>150</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>134</v>
+        <v>32</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>135</v>
+        <v>77</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C149" s="3">
-        <v>200.7</v>
+        <v>49</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B150" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B150" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="C150" s="3">
-        <v>200.8</v>
+        <v>200.7</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>35</v>
+        <v>136</v>
       </c>
       <c r="C151" s="3">
-        <v>200.7</v>
+        <v>200.8</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C152" s="3">
         <v>200.7</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C153" s="3" t="s">
-        <v>97</v>
+        <v>35</v>
+      </c>
+      <c r="C153" s="3">
+        <v>200.7</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>37</v>
+        <v>139</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>141</v>
+        <v>49</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>152</v>
+        <v>96</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>37</v>
+        <v>139</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>141</v>
+        <v>49</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>142</v>
+        <v>36</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C156" s="3">
-        <v>200.7</v>
+        <v>140</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>151</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>142</v>
+        <v>36</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C157" s="3">
-        <v>200.8</v>
+        <v>140</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>148</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B158" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B158" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C158" s="3" t="s">
-        <v>76</v>
+      <c r="C158" s="3">
+        <v>200.7</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B159" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B159" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C159" s="3" t="s">
-        <v>55</v>
+      <c r="C159" s="3">
+        <v>200.8</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D159">
+  <autoFilter ref="A1:D161">
     <sortState ref="A2:D272">
       <sortCondition ref="A1:A272"/>
     </sortState>

</xml_diff>

<commit_message>
additions to CFR method table. Edits to improve QL check and Method check functions
</commit_message>
<xml_diff>
--- a/3_13_2019_CFR_Methods.xlsx
+++ b/3_13_2019_CFR_Methods.xlsx
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$161</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="194">
   <si>
     <t>Char_Name</t>
   </si>
@@ -492,6 +489,123 @@
   </si>
   <si>
     <t>2340B</t>
+  </si>
+  <si>
+    <t>1,1-Dichloroethane</t>
+  </si>
+  <si>
+    <t>1,1-Dichloroethylene</t>
+  </si>
+  <si>
+    <t>1,1,1-Trichloroethane</t>
+  </si>
+  <si>
+    <t>1,1,2-Trichloroethane</t>
+  </si>
+  <si>
+    <t>1,1,2,2-Tetrachloroethane</t>
+  </si>
+  <si>
+    <t>1,2-Dichloroethane</t>
+  </si>
+  <si>
+    <t>1,2,4-Trichlorobenzene</t>
+  </si>
+  <si>
+    <t>2-Chloroethyl vinyl ether</t>
+  </si>
+  <si>
+    <t>1,2-Dichloropropane</t>
+  </si>
+  <si>
+    <t>2,4,6-Trichlorophenol</t>
+  </si>
+  <si>
+    <t>2,4-Dichlorophenol</t>
+  </si>
+  <si>
+    <t>2,4-Dimethylphenol</t>
+  </si>
+  <si>
+    <t>2,4-Dinitrophenol</t>
+  </si>
+  <si>
+    <t>2,4-Dinitrotoluene</t>
+  </si>
+  <si>
+    <t>2,6-Dinitrotoluene</t>
+  </si>
+  <si>
+    <t>2-Chloronaphthalene</t>
+  </si>
+  <si>
+    <t>3,3'-Dichlorobenzidine</t>
+  </si>
+  <si>
+    <t>4,6-Dinitro-o-cresol</t>
+  </si>
+  <si>
+    <t>71-55-6</t>
+  </si>
+  <si>
+    <t>79-34-5</t>
+  </si>
+  <si>
+    <t>79-00-5</t>
+  </si>
+  <si>
+    <t>75-34-3</t>
+  </si>
+  <si>
+    <t>75-35-4</t>
+  </si>
+  <si>
+    <t>120-82-1</t>
+  </si>
+  <si>
+    <t>107-06-2</t>
+  </si>
+  <si>
+    <t>78-87-5</t>
+  </si>
+  <si>
+    <t>110-75-8</t>
+  </si>
+  <si>
+    <t>88-06-2</t>
+  </si>
+  <si>
+    <t>120-83-2</t>
+  </si>
+  <si>
+    <t>105-67-9</t>
+  </si>
+  <si>
+    <t>51-28-5</t>
+  </si>
+  <si>
+    <t>121-14-2</t>
+  </si>
+  <si>
+    <t>606-20-2</t>
+  </si>
+  <si>
+    <t>91-58-7</t>
+  </si>
+  <si>
+    <t>91-94-1</t>
+  </si>
+  <si>
+    <t>534-52-1</t>
+  </si>
+  <si>
+    <t>624.1</t>
+  </si>
+  <si>
+    <t>625.1</t>
+  </si>
+  <si>
+    <t>612</t>
   </si>
 </sst>
 </file>
@@ -832,11 +946,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E161"/>
+  <dimension ref="A1:E180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E155" sqref="E155"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,14 +980,14 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3">
-        <v>615</v>
+      <c r="A2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>191</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>48</v>
@@ -883,31 +997,31 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" t="s">
+        <v>174</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>50</v>
+        <v>191</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>49</v>
+      <c r="A4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4" t="s">
+        <v>175</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>149</v>
+        <v>191</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>48</v>
@@ -917,31 +1031,31 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>49</v>
+      <c r="A5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" t="s">
+        <v>176</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>52</v>
+        <v>191</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="3">
-        <v>200.7</v>
+      <c r="A6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>191</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>48</v>
@@ -951,14 +1065,14 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="3">
-        <v>200.8</v>
+      <c r="A7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>192</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>48</v>
@@ -968,31 +1082,31 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
+      <c r="A8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B8" t="s">
+        <v>178</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>54</v>
+        <v>193</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="3">
-        <v>350.1</v>
+      <c r="A9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>191</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>48</v>
@@ -1002,34 +1116,34 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>55</v>
+      <c r="A10" t="s">
+        <v>163</v>
+      </c>
+      <c r="B10" t="s">
+        <v>180</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>38</v>
+        <v>191</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>55</v>
+      <c r="A11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B11" t="s">
+        <v>182</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>39</v>
+        <v>192</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>143</v>
@@ -1037,16 +1151,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="C12" s="3">
+        <v>615</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>143</v>
@@ -1054,13 +1168,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>51</v>
@@ -1070,82 +1184,82 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>55</v>
+      <c r="A14" t="s">
+        <v>165</v>
+      </c>
+      <c r="B14" t="s">
+        <v>183</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>56</v>
+        <v>192</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>55</v>
+      <c r="A15" t="s">
+        <v>166</v>
+      </c>
+      <c r="B15" t="s">
+        <v>184</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>58</v>
+        <v>192</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>55</v>
+      <c r="A16" t="s">
+        <v>167</v>
+      </c>
+      <c r="B16" t="s">
+        <v>185</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>59</v>
+        <v>192</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>147</v>
+      <c r="A17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B17" t="s">
+        <v>186</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>192</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="3">
-        <v>200.7</v>
+      <c r="A18" t="s">
+        <v>169</v>
+      </c>
+      <c r="B18" t="s">
+        <v>187</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>192</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>48</v>
@@ -1155,14 +1269,14 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="3">
-        <v>200.8</v>
+      <c r="A19" t="s">
+        <v>162</v>
+      </c>
+      <c r="B19" t="s">
+        <v>181</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>191</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>48</v>
@@ -1172,14 +1286,14 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="3">
-        <v>200.9</v>
+      <c r="A20" t="s">
+        <v>170</v>
+      </c>
+      <c r="B20" t="s">
+        <v>188</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>192</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>48</v>
@@ -1189,31 +1303,31 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>61</v>
+      <c r="A21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B21" t="s">
+        <v>189</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>54</v>
+        <v>191</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="3">
-        <v>200.7</v>
+      <c r="A22" t="s">
+        <v>172</v>
+      </c>
+      <c r="B22" t="s">
+        <v>190</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>192</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>48</v>
@@ -1224,13 +1338,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="3">
-        <v>200.8</v>
+        <v>49</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>149</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>48</v>
@@ -1241,16 +1355,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="3">
-        <v>200.9</v>
+        <v>49</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>143</v>
@@ -1258,16 +1372,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>63</v>
+        <v>4</v>
+      </c>
+      <c r="C25" s="3">
+        <v>200.7</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>143</v>
@@ -1275,16 +1389,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>64</v>
+        <v>4</v>
+      </c>
+      <c r="C26" s="3">
+        <v>200.8</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>143</v>
@@ -1292,10 +1406,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>62</v>
+        <v>4</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>54</v>
@@ -1309,13 +1423,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C28" s="3">
-        <v>614</v>
+        <v>350.1</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>48</v>
@@ -1326,16 +1440,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="3">
-        <v>200.7</v>
+        <v>55</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>143</v>
@@ -1343,16 +1457,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="3">
-        <v>200.8</v>
+        <v>55</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>143</v>
@@ -1360,13 +1474,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>51</v>
@@ -1377,16 +1491,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C32" s="3">
-        <v>200.7</v>
+        <v>55</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>143</v>
@@ -1394,16 +1508,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" s="3">
-        <v>200.8</v>
+        <v>55</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>143</v>
@@ -1411,16 +1525,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>143</v>
@@ -1428,16 +1542,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" s="3">
-        <v>200.7</v>
+        <v>55</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>143</v>
@@ -1445,16 +1559,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="3">
-        <v>200.8</v>
+        <v>55</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>147</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>143</v>
@@ -1462,16 +1576,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>54</v>
+        <v>61</v>
+      </c>
+      <c r="C37" s="3">
+        <v>200.7</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>143</v>
@@ -1479,16 +1593,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
+      </c>
+      <c r="C38" s="3">
+        <v>200.8</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>143</v>
@@ -1496,13 +1610,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="C39" s="3">
-        <v>300</v>
+        <v>200.9</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>48</v>
@@ -1513,16 +1627,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>150</v>
+        <v>54</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>143</v>
@@ -1530,10 +1644,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C41" s="3">
         <v>200.7</v>
@@ -1547,10 +1661,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C42" s="3">
         <v>200.8</v>
@@ -1564,10 +1678,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C43" s="3">
         <v>200.9</v>
@@ -1581,10 +1695,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>63</v>
@@ -1598,33 +1712,33 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>145</v>
-      </c>
       <c r="D46" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>143</v>
@@ -1632,13 +1746,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>146</v>
+        <v>65</v>
+      </c>
+      <c r="C47" s="3">
+        <v>614</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>48</v>
@@ -1649,13 +1763,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>150</v>
+        <v>6</v>
+      </c>
+      <c r="C48" s="3">
+        <v>200.7</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>48</v>
@@ -1666,16 +1780,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>77</v>
+        <v>6</v>
+      </c>
+      <c r="C49" s="3">
+        <v>200.8</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>143</v>
@@ -1683,13 +1797,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>51</v>
@@ -1700,10 +1814,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="C51" s="3">
         <v>200.7</v>
@@ -1717,10 +1831,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="C52" s="3">
         <v>200.8</v>
@@ -1734,16 +1848,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C53" s="3">
-        <v>200.9</v>
+        <v>68</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>143</v>
@@ -1751,13 +1865,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>80</v>
+        <v>7</v>
       </c>
       <c r="C54" s="3">
-        <v>218.2</v>
+        <v>200.7</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>48</v>
@@ -1768,16 +1882,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>54</v>
+        <v>7</v>
+      </c>
+      <c r="C55" s="3">
+        <v>200.8</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>143</v>
@@ -1785,16 +1899,16 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C56" s="3">
-        <v>200.7</v>
+        <v>7</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>143</v>
@@ -1802,16 +1916,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C57" s="3">
-        <v>200.8</v>
+        <v>7</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>143</v>
@@ -1819,16 +1933,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>81</v>
+        <v>8</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>54</v>
+        <v>9</v>
+      </c>
+      <c r="C58" s="3">
+        <v>300</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>143</v>
@@ -1836,16 +1950,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>83</v>
+        <v>150</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>143</v>
@@ -1853,13 +1967,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>153</v>
+        <v>72</v>
+      </c>
+      <c r="C60" s="3">
+        <v>200.7</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>48</v>
@@ -1870,13 +1984,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C61" s="3">
-        <v>200.7</v>
+        <v>200.8</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>48</v>
@@ -1887,13 +2001,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C62" s="3">
-        <v>200.8</v>
+        <v>200.9</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>48</v>
@@ -1904,16 +2018,16 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C63" s="3">
-        <v>200.9</v>
+        <v>72</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>143</v>
@@ -1921,10 +2035,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>54</v>
@@ -1936,18 +2050,18 @@
         <v>143</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>85</v>
+        <v>73</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>86</v>
+        <v>145</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>143</v>
@@ -1955,13 +2069,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>87</v>
+        <v>10</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C66" s="3">
-        <v>335.4</v>
+        <v>11</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>48</v>
@@ -1972,16 +2086,16 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>87</v>
+        <v>10</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>88</v>
+        <v>11</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>89</v>
+        <v>150</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>143</v>
@@ -1989,13 +2103,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>51</v>
@@ -2006,16 +2120,16 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>91</v>
+        <v>11</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>151</v>
+        <v>78</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>143</v>
@@ -2023,13 +2137,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>146</v>
+        <v>80</v>
+      </c>
+      <c r="C70" s="3">
+        <v>200.7</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>48</v>
@@ -2040,16 +2154,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>92</v>
+        <v>80</v>
+      </c>
+      <c r="C71" s="3">
+        <v>200.8</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>143</v>
@@ -2057,16 +2171,16 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
+      </c>
+      <c r="C72" s="3">
+        <v>200.9</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>143</v>
@@ -2074,16 +2188,16 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>94</v>
+        <v>80</v>
+      </c>
+      <c r="C73" s="3">
+        <v>218.2</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>143</v>
@@ -2091,13 +2205,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>51</v>
@@ -2108,13 +2222,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>151</v>
+        <v>12</v>
+      </c>
+      <c r="C75" s="3">
+        <v>200.7</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>48</v>
@@ -2125,13 +2239,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>146</v>
+        <v>12</v>
+      </c>
+      <c r="C76" s="3">
+        <v>200.8</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>48</v>
@@ -2142,16 +2256,16 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C77" s="3">
-        <v>353.2</v>
+        <v>12</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>143</v>
@@ -2159,16 +2273,16 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>143</v>
@@ -2176,13 +2290,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C79" s="3">
-        <v>200.7</v>
+        <v>49</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>48</v>
@@ -2193,13 +2307,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="C80" s="3">
-        <v>200.8</v>
+        <v>200.7</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>48</v>
@@ -2210,16 +2324,16 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>75</v>
+        <v>85</v>
+      </c>
+      <c r="C81" s="3">
+        <v>200.8</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>143</v>
@@ -2227,16 +2341,16 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>54</v>
+        <v>85</v>
+      </c>
+      <c r="C82" s="3">
+        <v>200.9</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>143</v>
@@ -2244,16 +2358,16 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C83" s="3">
-        <v>200.7</v>
+        <v>85</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>143</v>
@@ -2261,16 +2375,16 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C84" s="3">
-        <v>200.8</v>
+        <v>85</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>143</v>
@@ -2278,13 +2392,13 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="C85" s="3">
-        <v>200.9</v>
+        <v>335.4</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>48</v>
@@ -2295,13 +2409,13 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>51</v>
@@ -2312,13 +2426,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>51</v>
@@ -2329,16 +2443,16 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>101</v>
+        <v>14</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>54</v>
+        <v>151</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>143</v>
@@ -2346,13 +2460,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>103</v>
+        <v>15</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C89" s="3">
-        <v>200.7</v>
+        <v>16</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>48</v>
@@ -2363,16 +2477,16 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>103</v>
+        <v>15</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C90" s="3">
-        <v>200.8</v>
+        <v>16</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>143</v>
@@ -2380,13 +2494,13 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>103</v>
+        <v>15</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>51</v>
@@ -2397,13 +2511,13 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>103</v>
+        <v>15</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>51</v>
@@ -2414,16 +2528,16 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C93" s="3">
-        <v>614</v>
+        <v>16</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>143</v>
@@ -2431,13 +2545,13 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>105</v>
+        <v>17</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C94" s="3">
-        <v>200.7</v>
+        <v>97</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>151</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>48</v>
@@ -2448,13 +2562,13 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>105</v>
+        <v>18</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C95" s="3">
-        <v>200.8</v>
+        <v>49</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>48</v>
@@ -2465,13 +2579,13 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>105</v>
+        <v>18</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="C96" s="3">
-        <v>1638</v>
+        <v>353.2</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>48</v>
@@ -2482,16 +2596,16 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>105</v>
+        <v>18</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>143</v>
@@ -2499,16 +2613,16 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>54</v>
+        <v>100</v>
+      </c>
+      <c r="C98" s="3">
+        <v>200.7</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>143</v>
@@ -2516,13 +2630,13 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C99" s="3">
-        <v>245.1</v>
+        <v>200.8</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>48</v>
@@ -2533,16 +2647,16 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C100" s="3">
-        <v>245.2</v>
+        <v>100</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>143</v>
@@ -2550,16 +2664,16 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C101" s="3">
-        <v>245.7</v>
+        <v>100</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>143</v>
@@ -2567,13 +2681,13 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>108</v>
+        <v>102</v>
+      </c>
+      <c r="C102" s="3">
+        <v>200.7</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>48</v>
@@ -2584,16 +2698,16 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>109</v>
+        <v>102</v>
+      </c>
+      <c r="C103" s="3">
+        <v>200.8</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>143</v>
@@ -2601,13 +2715,13 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>22</v>
+        <v>101</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>151</v>
+        <v>102</v>
+      </c>
+      <c r="C104" s="3">
+        <v>200.9</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>48</v>
@@ -2618,16 +2732,16 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C105" s="3">
-        <v>200.7</v>
+        <v>102</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>143</v>
@@ -2635,16 +2749,16 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C106" s="3">
-        <v>200.8</v>
+        <v>102</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>143</v>
@@ -2652,10 +2766,10 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>54</v>
@@ -2669,10 +2783,10 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="C108" s="3">
         <v>200.7</v>
@@ -2686,10 +2800,10 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="C109" s="3">
         <v>200.8</v>
@@ -2703,13 +2817,13 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>51</v>
@@ -2720,16 +2834,16 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>24</v>
+        <v>103</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>114</v>
+        <v>19</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>146</v>
+        <v>54</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>143</v>
@@ -2737,16 +2851,16 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C112" s="3">
-        <v>10206</v>
+        <v>614</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>143</v>
@@ -2754,16 +2868,16 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>115</v>
+        <v>21</v>
+      </c>
+      <c r="C113" s="3">
+        <v>200.7</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>143</v>
@@ -2771,16 +2885,16 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>116</v>
+        <v>21</v>
+      </c>
+      <c r="C114" s="3">
+        <v>200.8</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>143</v>
@@ -2788,13 +2902,13 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>146</v>
+        <v>21</v>
+      </c>
+      <c r="C115" s="3">
+        <v>1638</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>48</v>
@@ -2805,16 +2919,16 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C116" s="3">
-        <v>353.2</v>
+        <v>21</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>143</v>
@@ -2822,13 +2936,13 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>117</v>
+        <v>54</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>51</v>
@@ -2839,16 +2953,16 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C118" s="3" t="s">
-        <v>119</v>
+        <v>107</v>
+      </c>
+      <c r="C118" s="3">
+        <v>245.1</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>143</v>
@@ -2856,13 +2970,13 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="C119" s="3">
-        <v>614</v>
+        <v>245.2</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>48</v>
@@ -2873,13 +2987,13 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>43</v>
+        <v>106</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C120" s="3" t="s">
-        <v>152</v>
+        <v>107</v>
+      </c>
+      <c r="C120" s="3">
+        <v>245.7</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>48</v>
@@ -2890,16 +3004,16 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>43</v>
+        <v>106</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>49</v>
+        <v>107</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>143</v>
@@ -2907,16 +3021,16 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>43</v>
+        <v>106</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>49</v>
+        <v>107</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>143</v>
@@ -2924,13 +3038,13 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C123" s="3">
-        <v>420.1</v>
+        <v>110</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>151</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>48</v>
@@ -2941,13 +3055,13 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="C124" s="3">
-        <v>365.3</v>
+        <v>200.7</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>48</v>
@@ -2958,16 +3072,16 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C125" s="3" t="s">
-        <v>121</v>
+        <v>23</v>
+      </c>
+      <c r="C125" s="3">
+        <v>200.8</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>143</v>
@@ -2975,13 +3089,13 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>122</v>
+        <v>54</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>51</v>
@@ -2992,10 +3106,10 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>29</v>
+        <v>112</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="C127" s="3">
         <v>200.7</v>
@@ -3009,13 +3123,13 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>29</v>
+        <v>112</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="C128" s="3">
-        <v>365.3</v>
+        <v>200.8</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>48</v>
@@ -3026,16 +3140,16 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C129" s="3">
-        <v>365.4</v>
+        <v>112</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>143</v>
@@ -3043,16 +3157,16 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>143</v>
@@ -3060,16 +3174,16 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C131" s="3" t="s">
-        <v>121</v>
+        <v>114</v>
+      </c>
+      <c r="C131" s="3">
+        <v>10206</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>143</v>
@@ -3077,13 +3191,13 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>29</v>
+        <v>114</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>51</v>
@@ -3094,16 +3208,16 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B133" s="2">
-        <v>2023695</v>
+        <v>24</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>145</v>
+        <v>116</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>143</v>
@@ -3111,13 +3225,13 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C134" s="3">
-        <v>200.7</v>
+        <v>49</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="D134" s="1" t="s">
         <v>48</v>
@@ -3128,13 +3242,13 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>129</v>
+        <v>49</v>
       </c>
       <c r="C135" s="3">
-        <v>200.8</v>
+        <v>353.2</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>48</v>
@@ -3145,16 +3259,16 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C136" s="3">
-        <v>200.9</v>
+        <v>49</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>143</v>
@@ -3162,13 +3276,13 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>129</v>
+        <v>49</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>64</v>
+        <v>119</v>
       </c>
       <c r="D137" s="1" t="s">
         <v>51</v>
@@ -3179,16 +3293,16 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>128</v>
+        <v>26</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C138" s="3" t="s">
-        <v>54</v>
+        <v>123</v>
+      </c>
+      <c r="C138" s="3">
+        <v>614</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>143</v>
@@ -3196,13 +3310,13 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>130</v>
+        <v>43</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C139" s="3">
-        <v>200.7</v>
+        <v>49</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="D139" s="1" t="s">
         <v>48</v>
@@ -3213,16 +3327,16 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>130</v>
+        <v>43</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C140" s="3">
-        <v>200.8</v>
+        <v>49</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>143</v>
@@ -3230,16 +3344,16 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>130</v>
+        <v>43</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C141" s="3">
-        <v>200.9</v>
+        <v>49</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>143</v>
@@ -3247,16 +3361,16 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>130</v>
+        <v>27</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C142" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
+      </c>
+      <c r="C142" s="3">
+        <v>420.1</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>143</v>
@@ -3264,13 +3378,13 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>30</v>
+        <v>126</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="C143" s="3">
-        <v>615</v>
+        <v>365.3</v>
       </c>
       <c r="D143" s="1" t="s">
         <v>48</v>
@@ -3281,13 +3395,13 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>30</v>
+        <v>126</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>50</v>
+        <v>121</v>
       </c>
       <c r="D144" s="1" t="s">
         <v>51</v>
@@ -3298,16 +3412,16 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>44</v>
+        <v>126</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>132</v>
+        <v>49</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>145</v>
+        <v>122</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>143</v>
@@ -3315,13 +3429,13 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C146" s="3" t="s">
-        <v>146</v>
+        <v>28</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C146" s="3">
+        <v>200.7</v>
       </c>
       <c r="D146" s="1" t="s">
         <v>48</v>
@@ -3332,13 +3446,13 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C147" s="3" t="s">
-        <v>150</v>
+        <v>28</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C147" s="3">
+        <v>365.3</v>
       </c>
       <c r="D147" s="1" t="s">
         <v>48</v>
@@ -3349,16 +3463,16 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C148" s="3" t="s">
-        <v>77</v>
+        <v>28</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C148" s="3">
+        <v>365.4</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>143</v>
@@ -3366,13 +3480,13 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>49</v>
+        <v>28</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>51</v>
@@ -3383,16 +3497,16 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>135</v>
+        <v>28</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C150" s="3">
-        <v>200.7</v>
+        <v>29</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>143</v>
@@ -3400,16 +3514,16 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>135</v>
+        <v>28</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C151" s="3">
-        <v>200.8</v>
+        <v>29</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E151" s="1" t="s">
         <v>143</v>
@@ -3417,13 +3531,13 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C152" s="3">
-        <v>200.7</v>
+        <v>127</v>
+      </c>
+      <c r="B152" s="2">
+        <v>2023695</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="D152" s="1" t="s">
         <v>48</v>
@@ -3434,10 +3548,10 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>35</v>
+        <v>129</v>
       </c>
       <c r="C153" s="3">
         <v>200.7</v>
@@ -3451,16 +3565,16 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C154" s="3" t="s">
-        <v>96</v>
+        <v>129</v>
+      </c>
+      <c r="C154" s="3">
+        <v>200.8</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E154" s="1" t="s">
         <v>143</v>
@@ -3468,16 +3582,16 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C155" s="3" t="s">
-        <v>154</v>
+        <v>129</v>
+      </c>
+      <c r="C155" s="3">
+        <v>200.9</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>143</v>
@@ -3485,16 +3599,16 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>36</v>
+        <v>128</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>151</v>
+        <v>64</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>143</v>
@@ -3502,16 +3616,16 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>36</v>
+        <v>128</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>148</v>
+        <v>54</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E157" s="1" t="s">
         <v>143</v>
@@ -3519,10 +3633,10 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C158" s="3">
         <v>200.7</v>
@@ -3536,10 +3650,10 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C159" s="3">
         <v>200.8</v>
@@ -3553,16 +3667,16 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C160" s="3" t="s">
-        <v>75</v>
+        <v>131</v>
+      </c>
+      <c r="C160" s="3">
+        <v>200.9</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E160" s="1" t="s">
         <v>143</v>
@@ -3570,10 +3684,10 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C161" s="3" t="s">
         <v>54</v>
@@ -3585,12 +3699,330 @@
         <v>143</v>
       </c>
     </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C162" s="3">
+        <v>615</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C169" s="3">
+        <v>200.7</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C170" s="3">
+        <v>200.8</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C171" s="3">
+        <v>200.7</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C172" s="3">
+        <v>200.7</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C177" s="3">
+        <v>200.7</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C178" s="3">
+        <v>200.8</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D161">
-    <sortState ref="A2:D272">
-      <sortCondition ref="A1:A272"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
sprucing up table in RMarkdown
</commit_message>
<xml_diff>
--- a/3_13_2019_CFR_Methods.xlsx
+++ b/3_13_2019_CFR_Methods.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Permit Job\R_Scripts\EDD_Data_QC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\R_Scripts\EDD_Data_QC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -949,8 +949,8 @@
   <dimension ref="A1:E180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added Chromium VI method to CFR method excel
</commit_message>
<xml_diff>
--- a/3_13_2019_CFR_Methods.xlsx
+++ b/3_13_2019_CFR_Methods.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="197">
   <si>
     <t>Char_Name</t>
   </si>
@@ -606,6 +606,15 @@
   </si>
   <si>
     <t>612</t>
+  </si>
+  <si>
+    <t>Chromium(VI)</t>
+  </si>
+  <si>
+    <t>218.6</t>
+  </si>
+  <si>
+    <t>18540-29-9</t>
   </si>
 </sst>
 </file>
@@ -946,11 +955,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E180"/>
+  <dimension ref="A1:E181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B108" sqref="B108"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2222,13 +2231,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C75" s="3">
-        <v>200.7</v>
+        <v>194</v>
+      </c>
+      <c r="B75" t="s">
+        <v>196</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>195</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>48</v>
@@ -2245,7 +2254,7 @@
         <v>12</v>
       </c>
       <c r="C76" s="3">
-        <v>200.8</v>
+        <v>200.7</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>48</v>
@@ -2261,11 +2270,11 @@
       <c r="B77" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C77" s="3" t="s">
-        <v>54</v>
+      <c r="C77" s="3">
+        <v>200.8</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>143</v>
@@ -2273,13 +2282,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>51</v>
@@ -2296,10 +2305,10 @@
         <v>49</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>153</v>
+        <v>83</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>143</v>
@@ -2307,13 +2316,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C80" s="3">
-        <v>200.7</v>
+        <v>49</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>48</v>
@@ -2330,7 +2339,7 @@
         <v>85</v>
       </c>
       <c r="C81" s="3">
-        <v>200.8</v>
+        <v>200.7</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>48</v>
@@ -2347,7 +2356,7 @@
         <v>85</v>
       </c>
       <c r="C82" s="3">
-        <v>200.9</v>
+        <v>200.8</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>48</v>
@@ -2363,11 +2372,11 @@
       <c r="B83" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C83" s="3" t="s">
-        <v>54</v>
+      <c r="C83" s="3">
+        <v>200.9</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>143</v>
@@ -2381,7 +2390,7 @@
         <v>85</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>51</v>
@@ -2392,16 +2401,16 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C85" s="3">
-        <v>335.4</v>
+        <v>85</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>143</v>
@@ -2414,11 +2423,11 @@
       <c r="B86" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C86" s="3" t="s">
-        <v>89</v>
+      <c r="C86" s="3">
+        <v>335.4</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>143</v>
@@ -2426,13 +2435,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>51</v>
@@ -2443,16 +2452,16 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>91</v>
+        <v>49</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>151</v>
+        <v>90</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>143</v>
@@ -2460,13 +2469,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>48</v>
@@ -2483,10 +2492,10 @@
         <v>16</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>92</v>
+        <v>146</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>143</v>
@@ -2500,7 +2509,7 @@
         <v>16</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>51</v>
@@ -2517,7 +2526,7 @@
         <v>16</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>51</v>
@@ -2534,7 +2543,7 @@
         <v>16</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>51</v>
@@ -2545,16 +2554,16 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>97</v>
+        <v>16</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>151</v>
+        <v>95</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>143</v>
@@ -2562,13 +2571,13 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>48</v>
@@ -2584,8 +2593,8 @@
       <c r="B96" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C96" s="3">
-        <v>353.2</v>
+      <c r="C96" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>48</v>
@@ -2601,8 +2610,8 @@
       <c r="B97" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C97" s="3" t="s">
-        <v>98</v>
+      <c r="C97" s="3">
+        <v>353.2</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>48</v>
@@ -2613,13 +2622,13 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>99</v>
+        <v>18</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C98" s="3">
-        <v>200.7</v>
+        <v>49</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>48</v>
@@ -2636,7 +2645,7 @@
         <v>100</v>
       </c>
       <c r="C99" s="3">
-        <v>200.8</v>
+        <v>200.7</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>48</v>
@@ -2652,11 +2661,11 @@
       <c r="B100" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C100" s="3" t="s">
-        <v>75</v>
+      <c r="C100" s="3">
+        <v>200.8</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>143</v>
@@ -2670,7 +2679,7 @@
         <v>100</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>51</v>
@@ -2681,16 +2690,16 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C102" s="3">
-        <v>200.7</v>
+        <v>100</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>143</v>
@@ -2704,7 +2713,7 @@
         <v>102</v>
       </c>
       <c r="C103" s="3">
-        <v>200.8</v>
+        <v>200.7</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>48</v>
@@ -2721,7 +2730,7 @@
         <v>102</v>
       </c>
       <c r="C104" s="3">
-        <v>200.9</v>
+        <v>200.8</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>48</v>
@@ -2737,11 +2746,11 @@
       <c r="B105" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C105" s="3" t="s">
-        <v>75</v>
+      <c r="C105" s="3">
+        <v>200.9</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>143</v>
@@ -2755,7 +2764,7 @@
         <v>102</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>51</v>
@@ -2772,7 +2781,7 @@
         <v>102</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>51</v>
@@ -2783,16 +2792,16 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C108" s="3">
-        <v>200.7</v>
+        <v>102</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>143</v>
@@ -2806,7 +2815,7 @@
         <v>19</v>
       </c>
       <c r="C109" s="3">
-        <v>200.8</v>
+        <v>200.7</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>48</v>
@@ -2822,11 +2831,11 @@
       <c r="B110" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C110" s="3" t="s">
-        <v>75</v>
+      <c r="C110" s="3">
+        <v>200.8</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>143</v>
@@ -2840,7 +2849,7 @@
         <v>19</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>51</v>
@@ -2851,16 +2860,16 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C112" s="3">
-        <v>614</v>
+        <v>19</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>143</v>
@@ -2868,13 +2877,13 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>105</v>
+        <v>20</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="C113" s="3">
-        <v>200.7</v>
+        <v>614</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>48</v>
@@ -2891,7 +2900,7 @@
         <v>21</v>
       </c>
       <c r="C114" s="3">
-        <v>200.8</v>
+        <v>200.7</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>48</v>
@@ -2908,7 +2917,7 @@
         <v>21</v>
       </c>
       <c r="C115" s="3">
-        <v>1638</v>
+        <v>200.8</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>48</v>
@@ -2924,11 +2933,11 @@
       <c r="B116" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C116" s="3" t="s">
-        <v>75</v>
+      <c r="C116" s="3">
+        <v>1638</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>143</v>
@@ -2942,7 +2951,7 @@
         <v>21</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>51</v>
@@ -2953,16 +2962,16 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C118" s="3">
-        <v>245.1</v>
+        <v>21</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>143</v>
@@ -2976,7 +2985,7 @@
         <v>107</v>
       </c>
       <c r="C119" s="3">
-        <v>245.2</v>
+        <v>245.1</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>48</v>
@@ -2993,7 +3002,7 @@
         <v>107</v>
       </c>
       <c r="C120" s="3">
-        <v>245.7</v>
+        <v>245.2</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>48</v>
@@ -3009,8 +3018,8 @@
       <c r="B121" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C121" s="3" t="s">
-        <v>108</v>
+      <c r="C121" s="3">
+        <v>245.7</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>48</v>
@@ -3027,10 +3036,10 @@
         <v>107</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>143</v>
@@ -3038,16 +3047,16 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>22</v>
+        <v>106</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>151</v>
+        <v>109</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>143</v>
@@ -3055,13 +3064,13 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>111</v>
+        <v>22</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C124" s="3">
-        <v>200.7</v>
+        <v>110</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>151</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>48</v>
@@ -3078,7 +3087,7 @@
         <v>23</v>
       </c>
       <c r="C125" s="3">
-        <v>200.8</v>
+        <v>200.7</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>48</v>
@@ -3094,11 +3103,11 @@
       <c r="B126" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C126" s="3" t="s">
-        <v>54</v>
+      <c r="C126" s="3">
+        <v>200.8</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>143</v>
@@ -3106,16 +3115,16 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C127" s="3">
-        <v>200.7</v>
+        <v>23</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>143</v>
@@ -3129,7 +3138,7 @@
         <v>113</v>
       </c>
       <c r="C128" s="3">
-        <v>200.8</v>
+        <v>200.7</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>48</v>
@@ -3145,11 +3154,11 @@
       <c r="B129" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C129" s="3" t="s">
-        <v>54</v>
+      <c r="C129" s="3">
+        <v>200.8</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>143</v>
@@ -3157,16 +3166,16 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>24</v>
+        <v>112</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>146</v>
+        <v>54</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>143</v>
@@ -3179,11 +3188,11 @@
       <c r="B131" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C131" s="3">
-        <v>10206</v>
+      <c r="C131" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>143</v>
@@ -3196,11 +3205,11 @@
       <c r="B132" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C132" s="3" t="s">
-        <v>115</v>
+      <c r="C132" s="3">
+        <v>10206</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>143</v>
@@ -3214,7 +3223,7 @@
         <v>114</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>51</v>
@@ -3225,16 +3234,16 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>49</v>
+        <v>114</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>146</v>
+        <v>116</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>143</v>
@@ -3247,8 +3256,8 @@
       <c r="B135" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C135" s="3">
-        <v>353.2</v>
+      <c r="C135" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>48</v>
@@ -3264,11 +3273,11 @@
       <c r="B136" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C136" s="3" t="s">
-        <v>117</v>
+      <c r="C136" s="3">
+        <v>353.2</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>143</v>
@@ -3276,13 +3285,13 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>118</v>
+        <v>25</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D137" s="1" t="s">
         <v>51</v>
@@ -3293,16 +3302,16 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>26</v>
+        <v>118</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C138" s="3">
-        <v>614</v>
+        <v>49</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>143</v>
@@ -3310,13 +3319,13 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C139" s="3" t="s">
-        <v>152</v>
+        <v>123</v>
+      </c>
+      <c r="C139" s="3">
+        <v>614</v>
       </c>
       <c r="D139" s="1" t="s">
         <v>48</v>
@@ -3333,10 +3342,10 @@
         <v>49</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>143</v>
@@ -3350,10 +3359,10 @@
         <v>49</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>143</v>
@@ -3361,16 +3370,16 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C142" s="3">
-        <v>420.1</v>
+      <c r="C142" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>143</v>
@@ -3378,13 +3387,13 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>126</v>
+        <v>27</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C143" s="3">
-        <v>365.3</v>
+        <v>420.1</v>
       </c>
       <c r="D143" s="1" t="s">
         <v>48</v>
@@ -3400,11 +3409,11 @@
       <c r="B144" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C144" s="3" t="s">
-        <v>121</v>
+      <c r="C144" s="3">
+        <v>365.3</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>143</v>
@@ -3418,7 +3427,7 @@
         <v>49</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D145" s="1" t="s">
         <v>51</v>
@@ -3429,16 +3438,16 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C146" s="3">
-        <v>200.7</v>
+        <v>126</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>143</v>
@@ -3452,7 +3461,7 @@
         <v>29</v>
       </c>
       <c r="C147" s="3">
-        <v>365.3</v>
+        <v>200.7</v>
       </c>
       <c r="D147" s="1" t="s">
         <v>48</v>
@@ -3469,7 +3478,7 @@
         <v>29</v>
       </c>
       <c r="C148" s="3">
-        <v>365.4</v>
+        <v>365.3</v>
       </c>
       <c r="D148" s="1" t="s">
         <v>48</v>
@@ -3485,11 +3494,11 @@
       <c r="B149" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C149" s="3" t="s">
-        <v>120</v>
+      <c r="C149" s="3">
+        <v>365.4</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>143</v>
@@ -3499,11 +3508,11 @@
       <c r="A150" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B150" s="1" t="s">
+      <c r="B150" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>51</v>
@@ -3520,7 +3529,7 @@
         <v>29</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>51</v>
@@ -3531,16 +3540,16 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B152" s="2">
-        <v>2023695</v>
+        <v>28</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>145</v>
+        <v>122</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E152" s="1" t="s">
         <v>143</v>
@@ -3548,13 +3557,13 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C153" s="3">
-        <v>200.7</v>
+        <v>127</v>
+      </c>
+      <c r="B153" s="2">
+        <v>2023695</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="D153" s="1" t="s">
         <v>48</v>
@@ -3571,7 +3580,7 @@
         <v>129</v>
       </c>
       <c r="C154" s="3">
-        <v>200.8</v>
+        <v>200.7</v>
       </c>
       <c r="D154" s="1" t="s">
         <v>48</v>
@@ -3588,7 +3597,7 @@
         <v>129</v>
       </c>
       <c r="C155" s="3">
-        <v>200.9</v>
+        <v>200.8</v>
       </c>
       <c r="D155" s="1" t="s">
         <v>48</v>
@@ -3604,11 +3613,11 @@
       <c r="B156" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C156" s="3" t="s">
-        <v>64</v>
+      <c r="C156" s="3">
+        <v>200.9</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>143</v>
@@ -3622,7 +3631,7 @@
         <v>129</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="D157" s="1" t="s">
         <v>51</v>
@@ -3633,16 +3642,16 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C158" s="3">
-        <v>200.7</v>
+        <v>129</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E158" s="1" t="s">
         <v>143</v>
@@ -3656,7 +3665,7 @@
         <v>131</v>
       </c>
       <c r="C159" s="3">
-        <v>200.8</v>
+        <v>200.7</v>
       </c>
       <c r="D159" s="1" t="s">
         <v>48</v>
@@ -3673,7 +3682,7 @@
         <v>131</v>
       </c>
       <c r="C160" s="3">
-        <v>200.9</v>
+        <v>200.8</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>48</v>
@@ -3689,11 +3698,11 @@
       <c r="B161" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C161" s="3" t="s">
-        <v>54</v>
+      <c r="C161" s="3">
+        <v>200.9</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E161" s="1" t="s">
         <v>143</v>
@@ -3701,16 +3710,16 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C162" s="3">
-        <v>615</v>
+        <v>131</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E162" s="1" t="s">
         <v>143</v>
@@ -3723,11 +3732,11 @@
       <c r="B163" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C163" s="3" t="s">
-        <v>50</v>
+      <c r="C163" s="3">
+        <v>615</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E163" s="1" t="s">
         <v>143</v>
@@ -3735,16 +3744,16 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>132</v>
+        <v>31</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>145</v>
+        <v>50</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>143</v>
@@ -3752,13 +3761,13 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>33</v>
+        <v>132</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D165" s="1" t="s">
         <v>48</v>
@@ -3775,7 +3784,7 @@
         <v>33</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D166" s="1" t="s">
         <v>48</v>
@@ -3792,10 +3801,10 @@
         <v>33</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>77</v>
+        <v>150</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E167" s="1" t="s">
         <v>143</v>
@@ -3803,13 +3812,13 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>133</v>
+        <v>32</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>134</v>
+        <v>77</v>
       </c>
       <c r="D168" s="1" t="s">
         <v>51</v>
@@ -3820,16 +3829,16 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C169" s="3">
-        <v>200.7</v>
+        <v>49</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E169" s="1" t="s">
         <v>143</v>
@@ -3843,7 +3852,7 @@
         <v>136</v>
       </c>
       <c r="C170" s="3">
-        <v>200.8</v>
+        <v>200.7</v>
       </c>
       <c r="D170" s="1" t="s">
         <v>48</v>
@@ -3854,13 +3863,13 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>34</v>
+        <v>136</v>
       </c>
       <c r="C171" s="3">
-        <v>200.7</v>
+        <v>200.8</v>
       </c>
       <c r="D171" s="1" t="s">
         <v>48</v>
@@ -3871,10 +3880,10 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C172" s="3">
         <v>200.7</v>
@@ -3888,16 +3897,16 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C173" s="3" t="s">
-        <v>96</v>
+        <v>35</v>
+      </c>
+      <c r="C173" s="3">
+        <v>200.7</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E173" s="1" t="s">
         <v>143</v>
@@ -3911,7 +3920,7 @@
         <v>49</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="D174" s="1" t="s">
         <v>51</v>
@@ -3922,16 +3931,16 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>36</v>
+        <v>139</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>140</v>
+        <v>49</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E175" s="1" t="s">
         <v>143</v>
@@ -3945,7 +3954,7 @@
         <v>140</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D176" s="1" t="s">
         <v>48</v>
@@ -3956,13 +3965,13 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>141</v>
+        <v>36</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C177" s="3">
-        <v>200.7</v>
+        <v>140</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>148</v>
       </c>
       <c r="D177" s="1" t="s">
         <v>48</v>
@@ -3979,7 +3988,7 @@
         <v>142</v>
       </c>
       <c r="C178" s="3">
-        <v>200.8</v>
+        <v>200.7</v>
       </c>
       <c r="D178" s="1" t="s">
         <v>48</v>
@@ -3995,11 +4004,11 @@
       <c r="B179" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C179" s="3" t="s">
-        <v>75</v>
+      <c r="C179" s="3">
+        <v>200.8</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E179" s="1" t="s">
         <v>143</v>
@@ -4013,12 +4022,29 @@
         <v>142</v>
       </c>
       <c r="C180" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C181" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D180" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E180" s="1" t="s">
+      <c r="D181" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E181" s="1" t="s">
         <v>143</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added CFR methods to list
</commit_message>
<xml_diff>
--- a/3_13_2019_CFR_Methods.xlsx
+++ b/3_13_2019_CFR_Methods.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="362">
   <si>
     <t>Char_Name</t>
   </si>
@@ -1071,6 +1071,48 @@
   </si>
   <si>
     <t>7440-09-7</t>
+  </si>
+  <si>
+    <t>Total suspended solids</t>
+  </si>
+  <si>
+    <t>2540-D</t>
+  </si>
+  <si>
+    <t>Total dissolved solids</t>
+  </si>
+  <si>
+    <t>2540-C</t>
+  </si>
+  <si>
+    <t>Dissolved oxygen (DO)</t>
+  </si>
+  <si>
+    <t>4500-O-G</t>
+  </si>
+  <si>
+    <t>Biochemical oxygen demand, standard conditions</t>
+  </si>
+  <si>
+    <t>5210-B</t>
+  </si>
+  <si>
+    <t>Chemical oxygen demand</t>
+  </si>
+  <si>
+    <t>5220-C</t>
+  </si>
+  <si>
+    <t>5220-D</t>
+  </si>
+  <si>
+    <t>Alkalinity, bicarbonate</t>
+  </si>
+  <si>
+    <t>Alkalinity, carbonate</t>
+  </si>
+  <si>
+    <t>Alkalinity, Hydroxide</t>
   </si>
 </sst>
 </file>
@@ -1444,8 +1486,8 @@
   <dimension ref="A1:E346"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C231" sqref="C231"/>
+      <pane ySplit="1" topLeftCell="A252" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D270" sqref="D270:E272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5921,67 +5963,139 @@
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A264"/>
+      <c r="A264" s="1" t="s">
+        <v>348</v>
+      </c>
       <c r="B264"/>
-      <c r="C264"/>
-      <c r="D264"/>
-      <c r="E264"/>
+      <c r="C264" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="D264" t="s">
+        <v>345</v>
+      </c>
+      <c r="E264" s="1" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A265"/>
+      <c r="A265" s="1" t="s">
+        <v>350</v>
+      </c>
       <c r="B265"/>
-      <c r="C265"/>
-      <c r="D265"/>
-      <c r="E265"/>
+      <c r="C265" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D265" t="s">
+        <v>345</v>
+      </c>
+      <c r="E265" s="1" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A266"/>
+      <c r="A266" s="1" t="s">
+        <v>352</v>
+      </c>
       <c r="B266"/>
-      <c r="C266"/>
-      <c r="D266"/>
-      <c r="E266"/>
+      <c r="C266" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D266" t="s">
+        <v>345</v>
+      </c>
+      <c r="E266" s="1" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A267"/>
+      <c r="A267" s="1" t="s">
+        <v>354</v>
+      </c>
       <c r="B267"/>
-      <c r="C267"/>
-      <c r="D267"/>
-      <c r="E267"/>
+      <c r="C267" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="D267" t="s">
+        <v>345</v>
+      </c>
+      <c r="E267" s="1" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A268"/>
+      <c r="A268" s="1" t="s">
+        <v>356</v>
+      </c>
       <c r="B268"/>
-      <c r="C268"/>
-      <c r="D268"/>
-      <c r="E268"/>
+      <c r="C268" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="D268" t="s">
+        <v>345</v>
+      </c>
+      <c r="E268" s="1" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A269"/>
+      <c r="A269" s="1" t="s">
+        <v>356</v>
+      </c>
       <c r="B269"/>
-      <c r="C269"/>
-      <c r="D269"/>
-      <c r="E269"/>
+      <c r="C269" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="D269" t="s">
+        <v>345</v>
+      </c>
+      <c r="E269" s="1" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A270"/>
+      <c r="A270" s="1" t="s">
+        <v>359</v>
+      </c>
       <c r="B270"/>
-      <c r="C270"/>
-      <c r="D270"/>
-      <c r="E270"/>
+      <c r="C270" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D270" t="s">
+        <v>345</v>
+      </c>
+      <c r="E270" s="1" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A271"/>
+      <c r="A271" s="1" t="s">
+        <v>360</v>
+      </c>
       <c r="B271"/>
-      <c r="C271"/>
-      <c r="D271"/>
-      <c r="E271"/>
+      <c r="C271" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D271" t="s">
+        <v>345</v>
+      </c>
+      <c r="E271" s="1" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A272"/>
+      <c r="A272" s="1" t="s">
+        <v>361</v>
+      </c>
       <c r="B272"/>
-      <c r="C272"/>
-      <c r="D272"/>
-      <c r="E272"/>
+      <c r="C272" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D272" t="s">
+        <v>345</v>
+      </c>
+      <c r="E272" s="1" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273"/>

</xml_diff>

<commit_message>
added a free cyanide method
</commit_message>
<xml_diff>
--- a/3_13_2019_CFR_Methods.xlsx
+++ b/3_13_2019_CFR_Methods.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$295</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1526" uniqueCount="418">
   <si>
     <t>Char_Name</t>
   </si>
@@ -1278,13 +1278,16 @@
   </si>
   <si>
     <t>Vinyl chloride</t>
+  </si>
+  <si>
+    <t>D4282</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1313,6 +1316,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1354,7 +1364,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1380,6 +1390,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1664,8 +1675,8 @@
   <dimension ref="A1:F342"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G327" sqref="G327"/>
+      <pane ySplit="1" topLeftCell="A311" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A334" sqref="A334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7190,11 +7201,19 @@
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A333"/>
+      <c r="A333" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="B333"/>
-      <c r="C333"/>
-      <c r="D333"/>
-      <c r="E333"/>
+      <c r="C333" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="D333" t="s">
+        <v>56</v>
+      </c>
+      <c r="E333" s="1" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334"/>

</xml_diff>

<commit_message>
adding "reissue" button and functionality
</commit_message>
<xml_diff>
--- a/3_13_2019_CFR_Methods.xlsx
+++ b/3_13_2019_CFR_Methods.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1676" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1684" uniqueCount="451">
   <si>
     <t>Char_Name</t>
   </si>
@@ -1377,6 +1377,9 @@
   </si>
   <si>
     <t>4500-S2(F)</t>
+  </si>
+  <si>
+    <t>365.4</t>
   </si>
 </sst>
 </file>
@@ -1786,11 +1789,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F371"/>
+  <dimension ref="A1:F373"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A362" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E372" sqref="E372"/>
+      <selection pane="bottomLeft" activeCell="C375" sqref="C375"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -7877,6 +7880,35 @@
         <v>142</v>
       </c>
     </row>
+    <row r="372" spans="1:5">
+      <c r="A372" t="s">
+        <v>125</v>
+      </c>
+      <c r="C372" t="s">
+        <v>450</v>
+      </c>
+      <c r="D372" t="s">
+        <v>48</v>
+      </c>
+      <c r="E372" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="373" spans="1:5">
+      <c r="A373" t="s">
+        <v>448</v>
+      </c>
+      <c r="B373"/>
+      <c r="C373" t="s">
+        <v>435</v>
+      </c>
+      <c r="D373" t="s">
+        <v>345</v>
+      </c>
+      <c r="E373" t="s">
+        <v>142</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E297">
     <sortState ref="A2:E369">

</xml_diff>